<commit_message>
formatted all times in PST and made sure they exported correctly
</commit_message>
<xml_diff>
--- a/Data/phytoplankton/2020/EMP_Phyto_Samples_2020_07.xlsx
+++ b/Data/phytoplankton/2020/EMP_Phyto_Samples_2020_07.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\AQUATICS\AQUATIC ARCHIVE\DATA ARCHIVES\CALIFORNIA\CDWR\Phytoplankton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\SMSCG\Data\phytoplankton\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72022F8B-A00C-4595-868D-83C7AA93CCC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58D552E-AC0F-45B9-9F3F-39F3EE8865AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="19200" windowHeight="10200" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Info" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="286">
   <si>
     <t>Aphanizomenon sp.</t>
   </si>
@@ -803,9 +803,6 @@
     <t>BSA.07-23</t>
   </si>
   <si>
-    <t xml:space="preserve"> 7/14/2020</t>
-  </si>
-  <si>
     <t>EZ6</t>
   </si>
   <si>
@@ -1533,51 +1530,51 @@
   <dimension ref="A1:BN330"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B273" sqref="B273:B275"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="9" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" style="37" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" style="11" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="12.26953125" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1796875" style="8" customWidth="1"/>
     <col min="15" max="15" width="38" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" style="9" customWidth="1"/>
-    <col min="18" max="18" width="28.5703125" style="9" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" style="19" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" style="19" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="5" customWidth="1"/>
-    <col min="22" max="24" width="10.42578125" style="9" customWidth="1"/>
-    <col min="25" max="25" width="16.5703125" style="19" customWidth="1"/>
-    <col min="26" max="27" width="12.140625" style="8" customWidth="1"/>
-    <col min="28" max="28" width="39.85546875" style="23" customWidth="1"/>
-    <col min="29" max="29" width="34.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="10.7109375" style="24" customWidth="1"/>
-    <col min="32" max="32" width="10.7109375" style="23" customWidth="1"/>
-    <col min="33" max="33" width="10.7109375" style="11" customWidth="1"/>
-    <col min="34" max="38" width="10.7109375" style="8" customWidth="1"/>
-    <col min="39" max="39" width="10.85546875" style="8" customWidth="1"/>
-    <col min="40" max="40" width="12.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="19.1796875" style="9" customWidth="1"/>
+    <col min="18" max="18" width="28.54296875" style="9" customWidth="1"/>
+    <col min="19" max="19" width="10.81640625" style="19" customWidth="1"/>
+    <col min="20" max="20" width="11.54296875" style="19" customWidth="1"/>
+    <col min="21" max="21" width="9.1796875" style="5" customWidth="1"/>
+    <col min="22" max="24" width="10.453125" style="9" customWidth="1"/>
+    <col min="25" max="25" width="16.54296875" style="19" customWidth="1"/>
+    <col min="26" max="27" width="12.1796875" style="8" customWidth="1"/>
+    <col min="28" max="28" width="39.81640625" style="23" customWidth="1"/>
+    <col min="29" max="29" width="34.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="10.7265625" style="24" customWidth="1"/>
+    <col min="32" max="32" width="10.7265625" style="23" customWidth="1"/>
+    <col min="33" max="33" width="10.7265625" style="11" customWidth="1"/>
+    <col min="34" max="38" width="10.7265625" style="8" customWidth="1"/>
+    <col min="39" max="39" width="10.81640625" style="8" customWidth="1"/>
+    <col min="40" max="40" width="12.1796875" style="31" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.7265625" style="34" bestFit="1" customWidth="1"/>
     <col min="42" max="50" width="15" style="34" bestFit="1" customWidth="1"/>
     <col min="51" max="66" width="16" style="34" bestFit="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.140625" style="8"/>
+    <col min="67" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1777,7 +1774,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:66" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:66" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1869,7 +1866,7 @@
         <v>66.7</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="28"/>
       <c r="C3" s="29"/>
@@ -1899,7 +1896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="28"/>
       <c r="C4" s="29"/>
@@ -1929,7 +1926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -2033,7 +2030,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="28"/>
       <c r="C6" s="29"/>
@@ -2077,7 +2074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -2181,7 +2178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -2377,7 +2374,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
@@ -2469,7 +2466,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="28"/>
       <c r="C10" s="29"/>
@@ -2498,7 +2495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="28"/>
       <c r="C11" s="29"/>
@@ -2527,7 +2524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>7</v>
       </c>
@@ -2619,7 +2616,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="28"/>
       <c r="C13" s="29"/>
@@ -2648,7 +2645,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>7</v>
       </c>
@@ -2740,7 +2737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="28"/>
       <c r="C15" s="29"/>
@@ -2769,7 +2766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="28"/>
       <c r="C16" s="29"/>
@@ -2798,7 +2795,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="28"/>
       <c r="C17" s="29"/>
@@ -2827,7 +2824,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>7</v>
       </c>
@@ -2919,7 +2916,7 @@
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="28"/>
       <c r="C19" s="29"/>
@@ -2947,7 +2944,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="28"/>
       <c r="C20" s="29"/>
@@ -2975,7 +2972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>7</v>
       </c>
@@ -3067,7 +3064,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="28"/>
       <c r="C22" s="29"/>
@@ -3096,7 +3093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
@@ -3125,7 +3122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>7</v>
       </c>
@@ -3229,7 +3226,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
@@ -3271,7 +3268,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>7</v>
       </c>
@@ -3375,7 +3372,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>7</v>
       </c>
@@ -3479,7 +3476,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
@@ -3520,7 +3517,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>7</v>
       </c>
@@ -3716,7 +3713,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>7</v>
       </c>
@@ -3823,7 +3820,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="28"/>
       <c r="C31" s="29"/>
@@ -3868,7 +3865,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="32" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>7</v>
       </c>
@@ -3992,7 +3989,7 @@
       <c r="BM32" s="51"/>
       <c r="BN32" s="51"/>
     </row>
-    <row r="33" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="39"/>
       <c r="C33" s="40"/>
@@ -4061,7 +4058,7 @@
       <c r="BM33" s="51"/>
       <c r="BN33" s="51"/>
     </row>
-    <row r="34" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="39"/>
       <c r="C34" s="40"/>
@@ -4130,7 +4127,7 @@
       <c r="BM34" s="51"/>
       <c r="BN34" s="51"/>
     </row>
-    <row r="35" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
         <v>7</v>
       </c>
@@ -4252,7 +4249,7 @@
       <c r="BM35" s="51"/>
       <c r="BN35" s="51"/>
     </row>
-    <row r="36" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
       <c r="B36" s="39"/>
       <c r="C36" s="40"/>
@@ -4319,7 +4316,7 @@
       <c r="BM36" s="51"/>
       <c r="BN36" s="51"/>
     </row>
-    <row r="37" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>7</v>
       </c>
@@ -4439,7 +4436,7 @@
       <c r="BM37" s="51"/>
       <c r="BN37" s="51"/>
     </row>
-    <row r="38" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
       <c r="B38" s="39"/>
       <c r="C38" s="40"/>
@@ -4503,7 +4500,7 @@
       <c r="BM38" s="51"/>
       <c r="BN38" s="51"/>
     </row>
-    <row r="39" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="39"/>
       <c r="C39" s="40"/>
@@ -4567,7 +4564,7 @@
       <c r="BM39" s="51"/>
       <c r="BN39" s="51"/>
     </row>
-    <row r="40" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
         <v>7</v>
       </c>
@@ -4687,7 +4684,7 @@
       <c r="BM40" s="51"/>
       <c r="BN40" s="51"/>
     </row>
-    <row r="41" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A41" s="19"/>
       <c r="B41" s="39"/>
       <c r="C41" s="40"/>
@@ -4752,7 +4749,7 @@
       <c r="BM41" s="51"/>
       <c r="BN41" s="51"/>
     </row>
-    <row r="42" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A42" s="19"/>
       <c r="B42" s="39"/>
       <c r="C42" s="40"/>
@@ -4817,7 +4814,7 @@
       <c r="BM42" s="51"/>
       <c r="BN42" s="51"/>
     </row>
-    <row r="43" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A43" s="19" t="s">
         <v>7</v>
       </c>
@@ -4939,7 +4936,7 @@
       <c r="BM43" s="51"/>
       <c r="BN43" s="51"/>
     </row>
-    <row r="44" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>7</v>
       </c>
@@ -5061,7 +5058,7 @@
       <c r="BM44" s="51"/>
       <c r="BN44" s="51"/>
     </row>
-    <row r="45" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="39"/>
       <c r="C45" s="40"/>
@@ -5129,7 +5126,7 @@
       <c r="BM45" s="51"/>
       <c r="BN45" s="51"/>
     </row>
-    <row r="46" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>7</v>
       </c>
@@ -5257,7 +5254,7 @@
       <c r="BM46" s="51"/>
       <c r="BN46" s="51"/>
     </row>
-    <row r="47" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
       <c r="B47" s="39"/>
       <c r="C47" s="40"/>
@@ -5331,7 +5328,7 @@
       <c r="BM47" s="51"/>
       <c r="BN47" s="51"/>
     </row>
-    <row r="48" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A48" s="19" t="s">
         <v>7</v>
       </c>
@@ -5459,7 +5456,7 @@
       <c r="BM48" s="51"/>
       <c r="BN48" s="51"/>
     </row>
-    <row r="49" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A49" s="19" t="s">
         <v>7</v>
       </c>
@@ -5655,7 +5652,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="50" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A50" s="19" t="s">
         <v>7</v>
       </c>
@@ -5781,7 +5778,7 @@
       <c r="BM50" s="51"/>
       <c r="BN50" s="51"/>
     </row>
-    <row r="51" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A51" s="19"/>
       <c r="B51" s="39"/>
       <c r="C51" s="40"/>
@@ -5853,7 +5850,7 @@
       <c r="BM51" s="51"/>
       <c r="BN51" s="51"/>
     </row>
-    <row r="52" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>7</v>
       </c>
@@ -5945,7 +5942,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="53" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
       <c r="B53" s="28"/>
       <c r="C53" s="29"/>
@@ -5974,7 +5971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
       <c r="B54" s="28"/>
       <c r="C54" s="29"/>
@@ -6003,7 +6000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>7</v>
       </c>
@@ -6107,7 +6104,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="56" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
       <c r="B56" s="28"/>
       <c r="C56" s="29"/>
@@ -6149,7 +6146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
         <v>7</v>
       </c>
@@ -6253,7 +6250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
         <v>7</v>
       </c>
@@ -6449,7 +6446,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="59" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A59" s="19" t="s">
         <v>7</v>
       </c>
@@ -6645,7 +6642,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="60" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>7</v>
       </c>
@@ -6737,7 +6734,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="61" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
       <c r="B61" s="28"/>
       <c r="C61" s="29"/>
@@ -6769,7 +6766,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="62" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
       <c r="B62" s="28"/>
       <c r="C62" s="29"/>
@@ -6801,7 +6798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>7</v>
       </c>
@@ -6890,7 +6887,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="64" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A64" s="9"/>
       <c r="B64" s="28"/>
       <c r="C64" s="29"/>
@@ -6918,7 +6915,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="65" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>7</v>
       </c>
@@ -7013,7 +7010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
         <v>7</v>
       </c>
@@ -7114,7 +7111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A67" s="9"/>
       <c r="B67" s="28"/>
       <c r="C67" s="29"/>
@@ -7156,7 +7153,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="68" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>7</v>
       </c>
@@ -7257,7 +7254,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="69" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A69" s="9"/>
       <c r="B69" s="28"/>
       <c r="C69" s="29"/>
@@ -7299,7 +7296,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="70" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>7</v>
       </c>
@@ -7400,7 +7397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>7</v>
       </c>
@@ -7593,7 +7590,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="72" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>7</v>
       </c>
@@ -7694,7 +7691,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="73" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="28"/>
       <c r="C73" s="29"/>
@@ -7736,7 +7733,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="74" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
         <v>7</v>
       </c>
@@ -7932,7 +7929,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="75" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A75" s="19" t="s">
         <v>7</v>
       </c>
@@ -8054,7 +8051,7 @@
       <c r="BM75" s="51"/>
       <c r="BN75" s="51"/>
     </row>
-    <row r="76" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A76" s="19"/>
       <c r="B76" s="39"/>
       <c r="C76" s="40"/>
@@ -8121,7 +8118,7 @@
       <c r="BM76" s="51"/>
       <c r="BN76" s="51"/>
     </row>
-    <row r="77" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A77" s="19"/>
       <c r="B77" s="39"/>
       <c r="C77" s="40"/>
@@ -8188,7 +8185,7 @@
       <c r="BM77" s="51"/>
       <c r="BN77" s="51"/>
     </row>
-    <row r="78" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A78" s="19" t="s">
         <v>7</v>
       </c>
@@ -8308,7 +8305,7 @@
       <c r="BM78" s="51"/>
       <c r="BN78" s="51"/>
     </row>
-    <row r="79" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A79" s="19"/>
       <c r="B79" s="39"/>
       <c r="C79" s="40"/>
@@ -8373,7 +8370,7 @@
       <c r="BM79" s="51"/>
       <c r="BN79" s="51"/>
     </row>
-    <row r="80" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A80" s="19" t="s">
         <v>7</v>
       </c>
@@ -8493,7 +8490,7 @@
       <c r="BM80" s="51"/>
       <c r="BN80" s="51"/>
     </row>
-    <row r="81" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A81" s="19"/>
       <c r="B81" s="39"/>
       <c r="C81" s="40"/>
@@ -8558,7 +8555,7 @@
       <c r="BM81" s="51"/>
       <c r="BN81" s="51"/>
     </row>
-    <row r="82" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A82" s="19" t="s">
         <v>7</v>
       </c>
@@ -8678,7 +8675,7 @@
       <c r="BM82" s="51"/>
       <c r="BN82" s="51"/>
     </row>
-    <row r="83" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A83" s="19"/>
       <c r="B83" s="39"/>
       <c r="C83" s="40"/>
@@ -8743,7 +8740,7 @@
       <c r="BM83" s="51"/>
       <c r="BN83" s="51"/>
     </row>
-    <row r="84" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A84" s="19"/>
       <c r="B84" s="39"/>
       <c r="C84" s="40"/>
@@ -8808,7 +8805,7 @@
       <c r="BM84" s="51"/>
       <c r="BN84" s="51"/>
     </row>
-    <row r="85" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A85" s="19"/>
       <c r="B85" s="39"/>
       <c r="C85" s="40"/>
@@ -8873,7 +8870,7 @@
       <c r="BM85" s="51"/>
       <c r="BN85" s="51"/>
     </row>
-    <row r="86" spans="1:66" s="46" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:66" s="46" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="19" t="s">
         <v>7</v>
       </c>
@@ -8993,7 +8990,7 @@
       <c r="BM86" s="51"/>
       <c r="BN86" s="51"/>
     </row>
-    <row r="87" spans="1:66" s="46" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:66" s="46" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="19"/>
       <c r="B87" s="39"/>
       <c r="C87" s="40"/>
@@ -9058,7 +9055,7 @@
       <c r="BM87" s="51"/>
       <c r="BN87" s="51"/>
     </row>
-    <row r="88" spans="1:66" s="46" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:66" s="46" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="19"/>
       <c r="B88" s="39"/>
       <c r="C88" s="40"/>
@@ -9123,7 +9120,7 @@
       <c r="BM88" s="51"/>
       <c r="BN88" s="51"/>
     </row>
-    <row r="89" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A89" s="19" t="s">
         <v>7</v>
       </c>
@@ -9243,7 +9240,7 @@
       <c r="BM89" s="51"/>
       <c r="BN89" s="51"/>
     </row>
-    <row r="90" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A90" s="19"/>
       <c r="B90" s="39"/>
       <c r="C90" s="40"/>
@@ -9308,7 +9305,7 @@
       <c r="BM90" s="51"/>
       <c r="BN90" s="51"/>
     </row>
-    <row r="91" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A91" s="19"/>
       <c r="B91" s="39"/>
       <c r="C91" s="40"/>
@@ -9373,7 +9370,7 @@
       <c r="BM91" s="51"/>
       <c r="BN91" s="51"/>
     </row>
-    <row r="92" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A92" s="19" t="s">
         <v>7</v>
       </c>
@@ -9569,7 +9566,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="93" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
         <v>7</v>
       </c>
@@ -9670,7 +9667,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A94" s="9"/>
       <c r="B94" s="28"/>
       <c r="C94" s="29"/>
@@ -9708,7 +9705,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="95" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A95" s="9"/>
       <c r="B95" s="28"/>
       <c r="C95" s="29"/>
@@ -9746,7 +9743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
         <v>7</v>
       </c>
@@ -9838,7 +9835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A97" s="9"/>
       <c r="B97" s="28"/>
       <c r="C97" s="29"/>
@@ -9867,7 +9864,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="98" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A98" s="9"/>
       <c r="B98" s="28"/>
       <c r="C98" s="29"/>
@@ -9896,7 +9893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="s">
         <v>7</v>
       </c>
@@ -9991,7 +9988,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="100" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A100" s="9"/>
       <c r="B100" s="28"/>
       <c r="C100" s="29"/>
@@ -10023,7 +10020,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A101" s="9"/>
       <c r="B101" s="28"/>
       <c r="C101" s="29"/>
@@ -10055,7 +10052,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="102" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A102" s="9"/>
       <c r="B102" s="28"/>
       <c r="C102" s="29"/>
@@ -10087,7 +10084,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="s">
         <v>7</v>
       </c>
@@ -10179,7 +10176,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A104" s="9"/>
       <c r="B104" s="28"/>
       <c r="C104" s="29"/>
@@ -10208,7 +10205,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="105" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A105" s="9"/>
       <c r="B105" s="28"/>
       <c r="C105" s="29"/>
@@ -10237,7 +10234,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="106" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A106" s="9" t="s">
         <v>7</v>
       </c>
@@ -10329,7 +10326,7 @@
         <v>38.9</v>
       </c>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A107" s="9"/>
       <c r="B107" s="28"/>
       <c r="C107" s="29"/>
@@ -10358,7 +10355,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A108" s="9"/>
       <c r="B108" s="28"/>
       <c r="C108" s="29"/>
@@ -10387,7 +10384,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A109" s="9" t="s">
         <v>7</v>
       </c>
@@ -10479,7 +10476,7 @@
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A110" s="9"/>
       <c r="B110" s="28"/>
       <c r="C110" s="29"/>
@@ -10507,7 +10504,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A111" s="9"/>
       <c r="B111" s="28"/>
       <c r="C111" s="29"/>
@@ -10535,7 +10532,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="112" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:43" ht="13" x14ac:dyDescent="0.3">
       <c r="A112" s="9" t="s">
         <v>7</v>
       </c>
@@ -10627,7 +10624,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="113" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A113" s="9" t="s">
         <v>7</v>
       </c>
@@ -10731,7 +10728,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="114" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A114" s="9"/>
       <c r="B114" s="28"/>
       <c r="C114" s="29"/>
@@ -10773,7 +10770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A115" s="9" t="s">
         <v>7</v>
       </c>
@@ -10877,7 +10874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A116" s="9" t="s">
         <v>7</v>
       </c>
@@ -11073,7 +11070,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="117" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A117" s="9" t="s">
         <v>7</v>
       </c>
@@ -11174,7 +11171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A118" s="9"/>
       <c r="B118" s="28"/>
       <c r="C118" s="29"/>
@@ -11213,7 +11210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A119" s="19" t="s">
         <v>7</v>
       </c>
@@ -11341,7 +11338,7 @@
       <c r="BM119" s="51"/>
       <c r="BN119" s="51"/>
     </row>
-    <row r="120" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A120" s="19" t="s">
         <v>7</v>
       </c>
@@ -11537,7 +11534,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="121" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A121" s="9" t="s">
         <v>7</v>
       </c>
@@ -11548,7 +11545,7 @@
         <v>0.5625</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E121" s="9">
         <v>3</v>
@@ -11629,7 +11626,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="122" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A122" s="9"/>
       <c r="B122" s="28"/>
       <c r="C122" s="29"/>
@@ -11658,7 +11655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A123" s="9"/>
       <c r="B123" s="28"/>
       <c r="C123" s="29"/>
@@ -11678,7 +11675,7 @@
       <c r="AD123" s="16"/>
       <c r="AE123" s="13"/>
       <c r="AN123" s="38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AO123" s="34">
         <v>55.6</v>
@@ -11687,7 +11684,7 @@
         <v>55.6</v>
       </c>
     </row>
-    <row r="124" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A124" s="9"/>
       <c r="B124" s="28"/>
       <c r="C124" s="29"/>
@@ -11707,7 +11704,7 @@
       <c r="AD124" s="16"/>
       <c r="AE124" s="13"/>
       <c r="AN124" s="38" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AO124" s="34">
         <v>1</v>
@@ -11716,7 +11713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A125" s="9" t="s">
         <v>7</v>
       </c>
@@ -11727,7 +11724,7 @@
         <v>0.5625</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E125" s="9">
         <v>3</v>
@@ -11820,7 +11817,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="126" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A126" s="9"/>
       <c r="B126" s="28"/>
       <c r="C126" s="29"/>
@@ -11861,7 +11858,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="127" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A127" s="9" t="s">
         <v>7</v>
       </c>
@@ -11872,7 +11869,7 @@
         <v>0.5625</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E127" s="9">
         <v>3</v>
@@ -12057,7 +12054,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="128" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A128" s="9" t="s">
         <v>7</v>
       </c>
@@ -12149,7 +12146,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="129" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A129" s="9"/>
       <c r="B129" s="28"/>
       <c r="C129" s="29"/>
@@ -12177,7 +12174,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="130" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A130" s="9"/>
       <c r="B130" s="28"/>
       <c r="C130" s="29"/>
@@ -12205,7 +12202,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A131" s="9" t="s">
         <v>7</v>
       </c>
@@ -12297,7 +12294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A132" s="9"/>
       <c r="B132" s="28"/>
       <c r="C132" s="29"/>
@@ -12325,7 +12322,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="133" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A133" s="9"/>
       <c r="B133" s="28"/>
       <c r="C133" s="29"/>
@@ -12353,7 +12350,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="134" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A134" s="9" t="s">
         <v>7</v>
       </c>
@@ -12457,7 +12454,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="135" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A135" s="9"/>
       <c r="B135" s="28"/>
       <c r="C135" s="29"/>
@@ -12499,7 +12496,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="136" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A136" s="9" t="s">
         <v>7</v>
       </c>
@@ -12603,7 +12600,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="137" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A137" s="9" t="s">
         <v>7</v>
       </c>
@@ -12799,7 +12796,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="138" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A138" s="9" t="s">
         <v>7</v>
       </c>
@@ -12894,7 +12891,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A139" s="9"/>
       <c r="B139" s="28"/>
       <c r="C139" s="29"/>
@@ -12926,7 +12923,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="140" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A140" s="9" t="s">
         <v>7</v>
       </c>
@@ -13018,7 +13015,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="141" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A141" s="9"/>
       <c r="B141" s="28"/>
       <c r="C141" s="29"/>
@@ -13047,7 +13044,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="142" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A142" s="9" t="s">
         <v>7</v>
       </c>
@@ -13139,7 +13136,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="143" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A143" s="9"/>
       <c r="B143" s="28"/>
       <c r="C143" s="29"/>
@@ -13168,7 +13165,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="144" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A144" s="9" t="s">
         <v>7</v>
       </c>
@@ -13272,7 +13269,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="145" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A145" s="9"/>
       <c r="B145" s="28"/>
       <c r="C145" s="29"/>
@@ -13314,7 +13311,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="146" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A146" s="9" t="s">
         <v>7</v>
       </c>
@@ -13415,7 +13412,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="147" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A147" s="9" t="s">
         <v>7</v>
       </c>
@@ -13611,7 +13608,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="148" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A148" s="9" t="s">
         <v>7</v>
       </c>
@@ -13715,7 +13712,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="149" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A149" s="9"/>
       <c r="B149" s="28"/>
       <c r="C149" s="29"/>
@@ -13757,7 +13754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A150" s="9" t="s">
         <v>7</v>
       </c>
@@ -13861,7 +13858,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="151" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="s">
         <v>7</v>
       </c>
@@ -13965,7 +13962,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="152" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A152" s="9"/>
       <c r="B152" s="28"/>
       <c r="C152" s="29"/>
@@ -14007,7 +14004,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="153" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A153" s="9" t="s">
         <v>7</v>
       </c>
@@ -14111,7 +14108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A154" s="9" t="s">
         <v>7</v>
       </c>
@@ -14307,7 +14304,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="155" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A155" s="9" t="s">
         <v>7</v>
       </c>
@@ -14402,7 +14399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A156" s="9"/>
       <c r="B156" s="28"/>
       <c r="C156" s="29"/>
@@ -14435,7 +14432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A157" s="9" t="s">
         <v>7</v>
       </c>
@@ -14539,7 +14536,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="158" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A158" s="9"/>
       <c r="B158" s="28"/>
       <c r="C158" s="29"/>
@@ -14581,7 +14578,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="159" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A159" s="19" t="s">
         <v>7</v>
       </c>
@@ -14701,7 +14698,7 @@
       <c r="BM159" s="51"/>
       <c r="BN159" s="51"/>
     </row>
-    <row r="160" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A160" s="19"/>
       <c r="B160" s="39"/>
       <c r="C160" s="40"/>
@@ -14766,7 +14763,7 @@
       <c r="BM160" s="51"/>
       <c r="BN160" s="51"/>
     </row>
-    <row r="161" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A161" s="19" t="s">
         <v>7</v>
       </c>
@@ -14892,7 +14889,7 @@
       <c r="BM161" s="51"/>
       <c r="BN161" s="51"/>
     </row>
-    <row r="162" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A162" s="19"/>
       <c r="B162" s="39"/>
       <c r="C162" s="40"/>
@@ -14963,7 +14960,7 @@
       <c r="BM162" s="51"/>
       <c r="BN162" s="51"/>
     </row>
-    <row r="163" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A163" s="19" t="s">
         <v>7</v>
       </c>
@@ -15091,7 +15088,7 @@
       <c r="BM163" s="51"/>
       <c r="BN163" s="51"/>
     </row>
-    <row r="164" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A164" s="19"/>
       <c r="B164" s="39"/>
       <c r="C164" s="40"/>
@@ -15164,7 +15161,7 @@
       <c r="BM164" s="51"/>
       <c r="BN164" s="51"/>
     </row>
-    <row r="165" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A165" s="9" t="s">
         <v>7</v>
       </c>
@@ -15256,7 +15253,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="166" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A166" s="9"/>
       <c r="B166" s="28"/>
       <c r="C166" s="29"/>
@@ -15285,7 +15282,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="167" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A167" s="9"/>
       <c r="B167" s="28"/>
       <c r="C167" s="29"/>
@@ -15305,7 +15302,7 @@
       <c r="AD167" s="16"/>
       <c r="AE167" s="13"/>
       <c r="AN167" s="38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AO167" s="34">
         <v>27.8</v>
@@ -15314,7 +15311,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="168" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A168" s="9"/>
       <c r="B168" s="28"/>
       <c r="C168" s="29"/>
@@ -15334,7 +15331,7 @@
       <c r="AD168" s="16"/>
       <c r="AE168" s="13"/>
       <c r="AN168" s="38" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AO168" s="34">
         <v>1</v>
@@ -15343,7 +15340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A169" s="19" t="s">
         <v>7</v>
       </c>
@@ -15465,7 +15462,7 @@
       <c r="BM169" s="51"/>
       <c r="BN169" s="51"/>
     </row>
-    <row r="170" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A170" s="19"/>
       <c r="B170" s="39"/>
       <c r="C170" s="40"/>
@@ -15531,7 +15528,7 @@
       <c r="BM170" s="51"/>
       <c r="BN170" s="51"/>
     </row>
-    <row r="171" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A171" s="19"/>
       <c r="B171" s="39"/>
       <c r="C171" s="40"/>
@@ -15597,7 +15594,7 @@
       <c r="BM171" s="51"/>
       <c r="BN171" s="51"/>
     </row>
-    <row r="172" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A172" s="19" t="s">
         <v>7</v>
       </c>
@@ -15717,7 +15714,7 @@
       <c r="BM172" s="51"/>
       <c r="BN172" s="51"/>
     </row>
-    <row r="173" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A173" s="19"/>
       <c r="B173" s="39"/>
       <c r="C173" s="40"/>
@@ -15781,7 +15778,7 @@
       <c r="BM173" s="51"/>
       <c r="BN173" s="51"/>
     </row>
-    <row r="174" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A174" s="19"/>
       <c r="B174" s="39"/>
       <c r="C174" s="40"/>
@@ -15845,7 +15842,7 @@
       <c r="BM174" s="51"/>
       <c r="BN174" s="51"/>
     </row>
-    <row r="175" spans="1:66" s="46" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:66" s="46" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="19" t="s">
         <v>7</v>
       </c>
@@ -15965,7 +15962,7 @@
       <c r="BM175" s="51"/>
       <c r="BN175" s="51"/>
     </row>
-    <row r="176" spans="1:66" s="46" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:66" s="46" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="19"/>
       <c r="B176" s="39"/>
       <c r="C176" s="40"/>
@@ -16030,7 +16027,7 @@
       <c r="BM176" s="51"/>
       <c r="BN176" s="51"/>
     </row>
-    <row r="177" spans="1:66" s="46" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:66" s="46" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="19"/>
       <c r="B177" s="39"/>
       <c r="C177" s="40"/>
@@ -16095,7 +16092,7 @@
       <c r="BM177" s="51"/>
       <c r="BN177" s="51"/>
     </row>
-    <row r="178" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A178" s="19" t="s">
         <v>7</v>
       </c>
@@ -16215,7 +16212,7 @@
       <c r="BM178" s="51"/>
       <c r="BN178" s="51"/>
     </row>
-    <row r="179" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A179" s="19"/>
       <c r="B179" s="39"/>
       <c r="C179" s="40"/>
@@ -16280,7 +16277,7 @@
       <c r="BM179" s="51"/>
       <c r="BN179" s="51"/>
     </row>
-    <row r="180" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A180" s="19"/>
       <c r="B180" s="39"/>
       <c r="C180" s="40"/>
@@ -16345,7 +16342,7 @@
       <c r="BM180" s="51"/>
       <c r="BN180" s="51"/>
     </row>
-    <row r="181" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A181" s="19" t="s">
         <v>7</v>
       </c>
@@ -16473,7 +16470,7 @@
       <c r="BM181" s="51"/>
       <c r="BN181" s="51"/>
     </row>
-    <row r="182" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A182" s="19"/>
       <c r="B182" s="39"/>
       <c r="C182" s="40"/>
@@ -16546,7 +16543,7 @@
       <c r="BM182" s="51"/>
       <c r="BN182" s="51"/>
     </row>
-    <row r="183" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A183" s="19"/>
       <c r="B183" s="39"/>
       <c r="C183" s="40"/>
@@ -16619,7 +16616,7 @@
       <c r="BM183" s="51"/>
       <c r="BN183" s="51"/>
     </row>
-    <row r="184" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A184" s="19" t="s">
         <v>7</v>
       </c>
@@ -16739,7 +16736,7 @@
       <c r="BM184" s="51"/>
       <c r="BN184" s="51"/>
     </row>
-    <row r="185" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A185" s="9"/>
       <c r="B185" s="28"/>
       <c r="C185" s="29"/>
@@ -16767,7 +16764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A186" s="9"/>
       <c r="B186" s="28"/>
       <c r="C186" s="29"/>
@@ -16795,7 +16792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A187" s="19" t="s">
         <v>7</v>
       </c>
@@ -16923,7 +16920,7 @@
       <c r="BM187" s="51"/>
       <c r="BN187" s="51"/>
     </row>
-    <row r="188" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A188" s="19"/>
       <c r="B188" s="39"/>
       <c r="C188" s="40"/>
@@ -16996,7 +16993,7 @@
       <c r="BM188" s="51"/>
       <c r="BN188" s="51"/>
     </row>
-    <row r="189" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A189" s="19"/>
       <c r="B189" s="39"/>
       <c r="C189" s="40"/>
@@ -17069,7 +17066,7 @@
       <c r="BM189" s="51"/>
       <c r="BN189" s="51"/>
     </row>
-    <row r="190" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A190" s="19" t="s">
         <v>7</v>
       </c>
@@ -17189,7 +17186,7 @@
       <c r="BM190" s="51"/>
       <c r="BN190" s="51"/>
     </row>
-    <row r="191" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A191" s="19"/>
       <c r="B191" s="39"/>
       <c r="C191" s="40"/>
@@ -17254,7 +17251,7 @@
       <c r="BM191" s="51"/>
       <c r="BN191" s="51"/>
     </row>
-    <row r="192" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A192" s="19"/>
       <c r="B192" s="39"/>
       <c r="C192" s="40"/>
@@ -17319,7 +17316,7 @@
       <c r="BM192" s="51"/>
       <c r="BN192" s="51"/>
     </row>
-    <row r="193" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A193" s="19" t="s">
         <v>7</v>
       </c>
@@ -17439,7 +17436,7 @@
       <c r="BM193" s="51"/>
       <c r="BN193" s="51"/>
     </row>
-    <row r="194" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A194" s="19"/>
       <c r="B194" s="39"/>
       <c r="C194" s="40"/>
@@ -17503,7 +17500,7 @@
       <c r="BM194" s="51"/>
       <c r="BN194" s="51"/>
     </row>
-    <row r="195" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A195" s="19"/>
       <c r="B195" s="39"/>
       <c r="C195" s="40"/>
@@ -17567,7 +17564,7 @@
       <c r="BM195" s="51"/>
       <c r="BN195" s="51"/>
     </row>
-    <row r="196" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A196" s="19" t="s">
         <v>7</v>
       </c>
@@ -17687,7 +17684,7 @@
       <c r="BM196" s="51"/>
       <c r="BN196" s="51"/>
     </row>
-    <row r="197" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A197" s="19"/>
       <c r="B197" s="39"/>
       <c r="C197" s="40"/>
@@ -17752,7 +17749,7 @@
       <c r="BM197" s="51"/>
       <c r="BN197" s="51"/>
     </row>
-    <row r="198" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A198" s="19"/>
       <c r="B198" s="39"/>
       <c r="C198" s="40"/>
@@ -17817,7 +17814,7 @@
       <c r="BM198" s="51"/>
       <c r="BN198" s="51"/>
     </row>
-    <row r="199" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A199" s="19" t="s">
         <v>7</v>
       </c>
@@ -17945,7 +17942,7 @@
       <c r="BM199" s="51"/>
       <c r="BN199" s="51"/>
     </row>
-    <row r="200" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A200" s="19"/>
       <c r="B200" s="39"/>
       <c r="C200" s="40"/>
@@ -18017,7 +18014,7 @@
       <c r="BM200" s="51"/>
       <c r="BN200" s="51"/>
     </row>
-    <row r="201" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A201" s="19" t="s">
         <v>7</v>
       </c>
@@ -18145,7 +18142,7 @@
       <c r="BM201" s="51"/>
       <c r="BN201" s="51"/>
     </row>
-    <row r="202" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A202" s="19" t="s">
         <v>7</v>
       </c>
@@ -18273,7 +18270,7 @@
       <c r="BM202" s="51"/>
       <c r="BN202" s="51"/>
     </row>
-    <row r="203" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A203" s="19"/>
       <c r="B203" s="39"/>
       <c r="C203" s="40"/>
@@ -18347,7 +18344,7 @@
       <c r="BM203" s="51"/>
       <c r="BN203" s="51"/>
     </row>
-    <row r="204" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A204" s="19" t="s">
         <v>7</v>
       </c>
@@ -18473,7 +18470,7 @@
       <c r="BM204" s="51"/>
       <c r="BN204" s="51"/>
     </row>
-    <row r="205" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A205" s="19"/>
       <c r="B205" s="39"/>
       <c r="C205" s="40"/>
@@ -18545,7 +18542,7 @@
       <c r="BM205" s="51"/>
       <c r="BN205" s="51"/>
     </row>
-    <row r="206" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A206" s="19" t="s">
         <v>7</v>
       </c>
@@ -18673,7 +18670,7 @@
       <c r="BM206" s="51"/>
       <c r="BN206" s="51"/>
     </row>
-    <row r="207" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A207" s="19"/>
       <c r="B207" s="39"/>
       <c r="C207" s="40"/>
@@ -18747,7 +18744,7 @@
       <c r="BM207" s="51"/>
       <c r="BN207" s="51"/>
     </row>
-    <row r="208" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A208" s="19" t="s">
         <v>7</v>
       </c>
@@ -18867,7 +18864,7 @@
       <c r="BM208" s="51"/>
       <c r="BN208" s="51"/>
     </row>
-    <row r="209" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A209" s="19"/>
       <c r="B209" s="39"/>
       <c r="C209" s="40"/>
@@ -18932,7 +18929,7 @@
       <c r="BM209" s="51"/>
       <c r="BN209" s="51"/>
     </row>
-    <row r="210" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A210" s="19"/>
       <c r="B210" s="39"/>
       <c r="C210" s="40"/>
@@ -18997,7 +18994,7 @@
       <c r="BM210" s="51"/>
       <c r="BN210" s="51"/>
     </row>
-    <row r="211" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A211" s="19" t="s">
         <v>7</v>
       </c>
@@ -19117,7 +19114,7 @@
       <c r="BM211" s="51"/>
       <c r="BN211" s="51"/>
     </row>
-    <row r="212" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A212" s="19"/>
       <c r="B212" s="39"/>
       <c r="C212" s="40"/>
@@ -19183,7 +19180,7 @@
       <c r="BM212" s="51"/>
       <c r="BN212" s="51"/>
     </row>
-    <row r="213" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A213" s="19" t="s">
         <v>7</v>
       </c>
@@ -19303,7 +19300,7 @@
       <c r="BM213" s="51"/>
       <c r="BN213" s="51"/>
     </row>
-    <row r="214" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A214" s="19"/>
       <c r="B214" s="39"/>
       <c r="C214" s="40"/>
@@ -19369,7 +19366,7 @@
       <c r="BM214" s="51"/>
       <c r="BN214" s="51"/>
     </row>
-    <row r="215" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A215" s="19"/>
       <c r="B215" s="39"/>
       <c r="C215" s="40"/>
@@ -19435,7 +19432,7 @@
       <c r="BM215" s="51"/>
       <c r="BN215" s="51"/>
     </row>
-    <row r="216" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A216" s="19" t="s">
         <v>7</v>
       </c>
@@ -19559,7 +19556,7 @@
       <c r="BM216" s="51"/>
       <c r="BN216" s="51"/>
     </row>
-    <row r="217" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A217" s="9" t="s">
         <v>7</v>
       </c>
@@ -19663,7 +19660,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="218" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A218" s="9"/>
       <c r="B218" s="28"/>
       <c r="C218" s="29"/>
@@ -19704,7 +19701,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="219" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A219" s="19" t="s">
         <v>7</v>
       </c>
@@ -19900,7 +19897,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="220" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A220" s="19" t="s">
         <v>7</v>
       </c>
@@ -20028,7 +20025,7 @@
       <c r="BM220" s="51"/>
       <c r="BN220" s="51"/>
     </row>
-    <row r="221" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A221" s="19"/>
       <c r="B221" s="39"/>
       <c r="C221" s="40"/>
@@ -20102,7 +20099,7 @@
       <c r="BM221" s="51"/>
       <c r="BN221" s="51"/>
     </row>
-    <row r="222" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A222" s="9" t="s">
         <v>7</v>
       </c>
@@ -20194,7 +20191,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="223" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A223" s="9"/>
       <c r="B223" s="28"/>
       <c r="C223" s="29"/>
@@ -20224,7 +20221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A224" s="9" t="s">
         <v>7</v>
       </c>
@@ -20420,7 +20417,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="225" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A225" s="9" t="s">
         <v>7</v>
       </c>
@@ -20524,7 +20521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A226" s="9"/>
       <c r="B226" s="28"/>
       <c r="C226" s="29"/>
@@ -20566,7 +20563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A227" s="9" t="s">
         <v>7</v>
       </c>
@@ -20670,7 +20667,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="228" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A228" s="9" t="s">
         <v>7</v>
       </c>
@@ -20866,7 +20863,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="229" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A229" s="9" t="s">
         <v>7</v>
       </c>
@@ -20967,7 +20964,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="230" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A230" s="9"/>
       <c r="B230" s="28"/>
       <c r="C230" s="29"/>
@@ -21006,7 +21003,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="231" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A231" s="19" t="s">
         <v>7</v>
       </c>
@@ -21126,7 +21123,7 @@
       <c r="BM231" s="51"/>
       <c r="BN231" s="51"/>
     </row>
-    <row r="232" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A232" s="19"/>
       <c r="B232" s="39"/>
       <c r="C232" s="40"/>
@@ -21190,7 +21187,7 @@
       <c r="BM232" s="51"/>
       <c r="BN232" s="51"/>
     </row>
-    <row r="233" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A233" s="19"/>
       <c r="B233" s="39"/>
       <c r="C233" s="40"/>
@@ -21254,7 +21251,7 @@
       <c r="BM233" s="51"/>
       <c r="BN233" s="51"/>
     </row>
-    <row r="234" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A234" s="19" t="s">
         <v>7</v>
       </c>
@@ -21382,7 +21379,7 @@
       <c r="BM234" s="51"/>
       <c r="BN234" s="51"/>
     </row>
-    <row r="235" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A235" s="19" t="s">
         <v>7</v>
       </c>
@@ -21578,7 +21575,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="236" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A236" s="9" t="s">
         <v>7</v>
       </c>
@@ -21679,7 +21676,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="237" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A237" s="9"/>
       <c r="B237" s="28"/>
       <c r="C237" s="29"/>
@@ -21717,7 +21714,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="238" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A238" s="9" t="s">
         <v>7</v>
       </c>
@@ -21809,7 +21806,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="239" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A239" s="9"/>
       <c r="B239" s="28"/>
       <c r="C239" s="29"/>
@@ -21837,7 +21834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A240" s="9"/>
       <c r="B240" s="28"/>
       <c r="C240" s="29"/>
@@ -21865,7 +21862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A241" s="9" t="s">
         <v>7</v>
       </c>
@@ -21966,7 +21963,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="242" spans="1:66" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:66" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="9" t="s">
         <v>7</v>
       </c>
@@ -22162,7 +22159,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="243" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A243" s="19" t="s">
         <v>7</v>
       </c>
@@ -22290,7 +22287,7 @@
       <c r="BM243" s="51"/>
       <c r="BN243" s="51"/>
     </row>
-    <row r="244" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A244" s="19"/>
       <c r="B244" s="39"/>
       <c r="C244" s="40"/>
@@ -22364,7 +22361,7 @@
       <c r="BM244" s="51"/>
       <c r="BN244" s="51"/>
     </row>
-    <row r="245" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A245" s="19" t="s">
         <v>7</v>
       </c>
@@ -22492,7 +22489,7 @@
       <c r="BM245" s="51"/>
       <c r="BN245" s="51"/>
     </row>
-    <row r="246" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A246" s="19" t="s">
         <v>7</v>
       </c>
@@ -22688,7 +22685,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="247" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A247" s="19" t="s">
         <v>7</v>
       </c>
@@ -22816,7 +22813,7 @@
       <c r="BM247" s="51"/>
       <c r="BN247" s="51"/>
     </row>
-    <row r="248" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A248" s="19"/>
       <c r="B248" s="39"/>
       <c r="C248" s="40"/>
@@ -22890,7 +22887,7 @@
       <c r="BM248" s="51"/>
       <c r="BN248" s="51"/>
     </row>
-    <row r="249" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A249" s="9" t="s">
         <v>7</v>
       </c>
@@ -22982,7 +22979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="250" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A250" s="9"/>
       <c r="B250" s="28"/>
       <c r="C250" s="29"/>
@@ -23011,7 +23008,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="251" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A251" s="9" t="s">
         <v>7</v>
       </c>
@@ -23109,7 +23106,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="252" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A252" s="9"/>
       <c r="B252" s="28"/>
       <c r="C252" s="29"/>
@@ -23144,7 +23141,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="253" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A253" s="9" t="s">
         <v>7</v>
       </c>
@@ -23236,7 +23233,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="254" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A254" s="9" t="s">
         <v>7</v>
       </c>
@@ -23328,7 +23325,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="255" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A255" s="9"/>
       <c r="B255" s="28"/>
       <c r="C255" s="29"/>
@@ -23358,7 +23355,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="256" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A256" s="9" t="s">
         <v>7</v>
       </c>
@@ -23453,7 +23450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A257" s="9" t="s">
         <v>7</v>
       </c>
@@ -23649,7 +23646,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="258" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A258" s="19" t="s">
         <v>7</v>
       </c>
@@ -23769,7 +23766,7 @@
       <c r="BM258" s="51"/>
       <c r="BN258" s="51"/>
     </row>
-    <row r="259" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A259" s="19"/>
       <c r="B259" s="39"/>
       <c r="C259" s="40"/>
@@ -23834,7 +23831,7 @@
       <c r="BM259" s="51"/>
       <c r="BN259" s="51"/>
     </row>
-    <row r="260" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A260" s="19"/>
       <c r="B260" s="39"/>
       <c r="C260" s="40"/>
@@ -23899,7 +23896,7 @@
       <c r="BM260" s="51"/>
       <c r="BN260" s="51"/>
     </row>
-    <row r="261" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A261" s="19" t="s">
         <v>7</v>
       </c>
@@ -24019,7 +24016,7 @@
       <c r="BM261" s="51"/>
       <c r="BN261" s="51"/>
     </row>
-    <row r="262" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A262" s="19" t="s">
         <v>7</v>
       </c>
@@ -24215,18 +24212,18 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="263" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A263" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B263" s="28" t="s">
-        <v>257</v>
+      <c r="B263" s="28">
+        <v>44026</v>
       </c>
       <c r="C263" s="29">
         <v>0.46875</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E263" s="9">
         <v>3</v>
@@ -24307,7 +24304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A264" s="9"/>
       <c r="B264" s="28"/>
       <c r="C264" s="29"/>
@@ -24336,18 +24333,18 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="265" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A265" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B265" s="28" t="s">
-        <v>257</v>
+      <c r="B265" s="28">
+        <v>44026</v>
       </c>
       <c r="C265" s="29">
         <v>0.46875</v>
       </c>
       <c r="D265" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E265" s="9">
         <v>3</v>
@@ -24380,7 +24377,7 @@
         <v>579</v>
       </c>
       <c r="O265" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P265" s="8" t="s">
         <v>22</v>
@@ -24389,7 +24386,7 @@
         <v>105</v>
       </c>
       <c r="R265" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="S265" s="9"/>
       <c r="T265" s="20">
@@ -24428,7 +24425,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="266" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A266" s="9"/>
       <c r="B266" s="28"/>
       <c r="C266" s="29"/>
@@ -24457,7 +24454,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="267" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A267" s="9"/>
       <c r="B267" s="28"/>
       <c r="C267" s="29"/>
@@ -24486,18 +24483,18 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="268" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A268" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B268" s="28" t="s">
-        <v>257</v>
+      <c r="B268" s="28">
+        <v>44026</v>
       </c>
       <c r="C268" s="29">
         <v>0.46875</v>
       </c>
       <c r="D268" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E268" s="9">
         <v>3</v>
@@ -24530,7 +24527,7 @@
         <v>676</v>
       </c>
       <c r="O268" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P268" s="8" t="s">
         <v>22</v>
@@ -24539,7 +24536,7 @@
         <v>46</v>
       </c>
       <c r="R268" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="S268" s="9"/>
       <c r="T268" s="20">
@@ -24578,7 +24575,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="269" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A269" s="9"/>
       <c r="B269" s="28"/>
       <c r="C269" s="29"/>
@@ -24607,7 +24604,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="270" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A270" s="9"/>
       <c r="B270" s="28"/>
       <c r="C270" s="29"/>
@@ -24636,18 +24633,18 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="271" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A271" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B271" s="28" t="s">
-        <v>257</v>
+      <c r="B271" s="28">
+        <v>44026</v>
       </c>
       <c r="C271" s="29">
         <v>0.46875</v>
       </c>
       <c r="D271" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E271" s="9">
         <v>3</v>
@@ -24740,7 +24737,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="272" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A272" s="9"/>
       <c r="B272" s="28"/>
       <c r="C272" s="29"/>
@@ -24782,18 +24779,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A273" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B273" s="28" t="s">
-        <v>257</v>
+      <c r="B273" s="28">
+        <v>44026</v>
       </c>
       <c r="C273" s="29">
         <v>0.46875</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E273" s="9">
         <v>3</v>
@@ -24886,18 +24883,18 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="274" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A274" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B274" s="28" t="s">
-        <v>257</v>
+      <c r="B274" s="28">
+        <v>44026</v>
       </c>
       <c r="C274" s="29">
         <v>0.46875</v>
       </c>
       <c r="D274" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E274" s="9">
         <v>3</v>
@@ -25082,18 +25079,18 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="275" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A275" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B275" s="28" t="s">
-        <v>257</v>
+      <c r="B275" s="28">
+        <v>44026</v>
       </c>
       <c r="C275" s="29">
         <v>0.46875</v>
       </c>
       <c r="D275" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E275" s="9">
         <v>3</v>
@@ -25186,7 +25183,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="276" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A276" s="9"/>
       <c r="B276" s="28"/>
       <c r="C276" s="29"/>
@@ -25228,7 +25225,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="277" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A277" s="9" t="s">
         <v>7</v>
       </c>
@@ -25239,7 +25236,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="D277" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E277" s="9">
         <v>3</v>
@@ -25297,7 +25294,7 @@
         <v>5</v>
       </c>
       <c r="Z277" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA277" s="8" t="s">
         <v>91</v>
@@ -25332,7 +25329,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="278" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A278" s="9"/>
       <c r="B278" s="28"/>
       <c r="C278" s="29"/>
@@ -25373,7 +25370,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="279" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A279" s="9" t="s">
         <v>7</v>
       </c>
@@ -25384,7 +25381,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="D279" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E279" s="9">
         <v>3</v>
@@ -25417,13 +25414,13 @@
         <v>326</v>
       </c>
       <c r="O279" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P279" s="8" t="s">
         <v>22</v>
       </c>
       <c r="Q279" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R279" s="9" t="s">
         <v>51</v>
@@ -25442,14 +25439,14 @@
         <v>5</v>
       </c>
       <c r="Z279" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA279" s="8" t="s">
         <v>91</v>
       </c>
       <c r="AB279" s="11"/>
       <c r="AC279" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AD279" s="16">
         <v>1067.9203194713241</v>
@@ -25465,7 +25462,7 @@
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="280" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A280" s="9"/>
       <c r="B280" s="28"/>
       <c r="C280" s="29"/>
@@ -25494,7 +25491,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="281" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A281" s="9"/>
       <c r="B281" s="28"/>
       <c r="C281" s="29"/>
@@ -25523,7 +25520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="282" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A282" s="9" t="s">
         <v>7</v>
       </c>
@@ -25534,7 +25531,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="D282" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E282" s="9">
         <v>3</v>
@@ -25567,7 +25564,7 @@
         <v>425</v>
       </c>
       <c r="O282" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P282" s="8" t="s">
         <v>22</v>
@@ -25592,7 +25589,7 @@
         <v>5</v>
       </c>
       <c r="Z282" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA282" s="8" t="s">
         <v>91</v>
@@ -25615,7 +25612,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="283" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A283" s="9"/>
       <c r="B283" s="28"/>
       <c r="C283" s="29"/>
@@ -25643,7 +25640,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="284" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A284" s="9"/>
       <c r="B284" s="28"/>
       <c r="C284" s="29"/>
@@ -25671,7 +25668,7 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="285" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A285" s="9"/>
       <c r="B285" s="28"/>
       <c r="C285" s="29"/>
@@ -25699,7 +25696,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="286" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A286" s="9" t="s">
         <v>7</v>
       </c>
@@ -25710,7 +25707,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="D286" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E286" s="9">
         <v>3</v>
@@ -25768,7 +25765,7 @@
         <v>5</v>
       </c>
       <c r="Z286" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA286" s="8" t="s">
         <v>91</v>
@@ -25791,7 +25788,7 @@
         <v>66.7</v>
       </c>
     </row>
-    <row r="287" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A287" s="9"/>
       <c r="B287" s="28"/>
       <c r="C287" s="29"/>
@@ -25820,7 +25817,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="288" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A288" s="9"/>
       <c r="B288" s="28"/>
       <c r="C288" s="29"/>
@@ -25849,7 +25846,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="289" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A289" s="9" t="s">
         <v>7</v>
       </c>
@@ -25860,7 +25857,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="D289" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E289" s="9">
         <v>3</v>
@@ -25918,7 +25915,7 @@
         <v>5</v>
       </c>
       <c r="Z289" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA289" s="8" t="s">
         <v>91</v>
@@ -25947,7 +25944,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="290" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A290" s="9"/>
       <c r="B290" s="28"/>
       <c r="C290" s="29"/>
@@ -25983,7 +25980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="291" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A291" s="9" t="s">
         <v>7</v>
       </c>
@@ -25994,7 +25991,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="D291" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E291" s="9">
         <v>3</v>
@@ -26052,7 +26049,7 @@
         <v>5</v>
       </c>
       <c r="Z291" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA291" s="8" t="s">
         <v>91</v>
@@ -26075,7 +26072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="292" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:66" ht="13" x14ac:dyDescent="0.3">
       <c r="A292" s="9" t="s">
         <v>7</v>
       </c>
@@ -26086,7 +26083,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="D292" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E292" s="9">
         <v>3</v>
@@ -26150,7 +26147,7 @@
         <v>56</v>
       </c>
       <c r="Z292" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA292" s="8" t="s">
         <v>91</v>
@@ -26271,7 +26268,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="293" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A293" s="19" t="s">
         <v>7</v>
       </c>
@@ -26282,7 +26279,7 @@
         <v>0.57291666666666696</v>
       </c>
       <c r="D293" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E293" s="19">
         <v>3</v>
@@ -26342,7 +26339,7 @@
         <v>5</v>
       </c>
       <c r="Z293" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AA293" s="8" t="s">
         <v>91</v>
@@ -26391,7 +26388,7 @@
       <c r="BM293" s="51"/>
       <c r="BN293" s="51"/>
     </row>
-    <row r="294" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A294" s="19"/>
       <c r="B294" s="39"/>
       <c r="C294" s="40"/>
@@ -26456,7 +26453,7 @@
       <c r="BM294" s="51"/>
       <c r="BN294" s="51"/>
     </row>
-    <row r="295" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A295" s="19"/>
       <c r="B295" s="39"/>
       <c r="C295" s="40"/>
@@ -26521,7 +26518,7 @@
       <c r="BM295" s="51"/>
       <c r="BN295" s="51"/>
     </row>
-    <row r="296" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A296" s="19" t="s">
         <v>7</v>
       </c>
@@ -26532,7 +26529,7 @@
         <v>0.57291666666666696</v>
       </c>
       <c r="D296" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E296" s="19">
         <v>3</v>
@@ -26592,7 +26589,7 @@
         <v>5</v>
       </c>
       <c r="Z296" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AA296" s="8" t="s">
         <v>91</v>
@@ -26649,7 +26646,7 @@
       <c r="BM296" s="51"/>
       <c r="BN296" s="51"/>
     </row>
-    <row r="297" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A297" s="19"/>
       <c r="B297" s="39"/>
       <c r="C297" s="40"/>
@@ -26722,7 +26719,7 @@
       <c r="BM297" s="51"/>
       <c r="BN297" s="51"/>
     </row>
-    <row r="298" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A298" s="19" t="s">
         <v>7</v>
       </c>
@@ -26733,7 +26730,7 @@
         <v>0.57291666666666696</v>
       </c>
       <c r="D298" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E298" s="19">
         <v>3</v>
@@ -26793,7 +26790,7 @@
         <v>5</v>
       </c>
       <c r="Z298" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AA298" s="8" t="s">
         <v>91</v>
@@ -26842,7 +26839,7 @@
       <c r="BM298" s="51"/>
       <c r="BN298" s="51"/>
     </row>
-    <row r="299" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A299" s="19"/>
       <c r="B299" s="39"/>
       <c r="C299" s="40"/>
@@ -26907,7 +26904,7 @@
       <c r="BM299" s="51"/>
       <c r="BN299" s="51"/>
     </row>
-    <row r="300" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A300" s="19"/>
       <c r="B300" s="39"/>
       <c r="C300" s="40"/>
@@ -26972,7 +26969,7 @@
       <c r="BM300" s="51"/>
       <c r="BN300" s="51"/>
     </row>
-    <row r="301" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A301" s="19" t="s">
         <v>7</v>
       </c>
@@ -26983,7 +26980,7 @@
         <v>0.57291666666666696</v>
       </c>
       <c r="D301" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E301" s="19">
         <v>3</v>
@@ -27016,7 +27013,7 @@
         <v>749</v>
       </c>
       <c r="O301" s="45" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="P301" s="46" t="s">
         <v>22</v>
@@ -27043,7 +27040,7 @@
         <v>5</v>
       </c>
       <c r="Z301" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AA301" s="8" t="s">
         <v>91</v>
@@ -27092,7 +27089,7 @@
       <c r="BM301" s="51"/>
       <c r="BN301" s="51"/>
     </row>
-    <row r="302" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A302" s="19"/>
       <c r="B302" s="39"/>
       <c r="C302" s="40"/>
@@ -27157,7 +27154,7 @@
       <c r="BM302" s="51"/>
       <c r="BN302" s="51"/>
     </row>
-    <row r="303" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A303" s="19"/>
       <c r="B303" s="39"/>
       <c r="C303" s="40"/>
@@ -27222,7 +27219,7 @@
       <c r="BM303" s="51"/>
       <c r="BN303" s="51"/>
     </row>
-    <row r="304" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A304" s="19" t="s">
         <v>7</v>
       </c>
@@ -27233,7 +27230,7 @@
         <v>0.57291666666666696</v>
       </c>
       <c r="D304" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E304" s="19">
         <v>3</v>
@@ -27293,7 +27290,7 @@
         <v>5</v>
       </c>
       <c r="Z304" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AA304" s="8" t="s">
         <v>91</v>
@@ -27350,7 +27347,7 @@
       <c r="BM304" s="51"/>
       <c r="BN304" s="51"/>
     </row>
-    <row r="305" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A305" s="19" t="s">
         <v>7</v>
       </c>
@@ -27361,7 +27358,7 @@
         <v>0.57291666666666696</v>
       </c>
       <c r="D305" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E305" s="19">
         <v>3</v>
@@ -27425,7 +27422,7 @@
         <v>56</v>
       </c>
       <c r="Z305" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AA305" s="8" t="s">
         <v>91</v>
@@ -27546,7 +27543,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="306" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A306" s="19" t="s">
         <v>7</v>
       </c>
@@ -27557,7 +27554,7 @@
         <v>0.60069444444444442</v>
       </c>
       <c r="D306" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E306" s="19">
         <v>3</v>
@@ -27617,7 +27614,7 @@
         <v>5</v>
       </c>
       <c r="Z306" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA306" s="46" t="s">
         <v>91</v>
@@ -27666,7 +27663,7 @@
       <c r="BM306" s="51"/>
       <c r="BN306" s="51"/>
     </row>
-    <row r="307" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A307" s="19"/>
       <c r="B307" s="39"/>
       <c r="C307" s="40"/>
@@ -27731,7 +27728,7 @@
       <c r="BM307" s="51"/>
       <c r="BN307" s="51"/>
     </row>
-    <row r="308" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A308" s="19" t="s">
         <v>7</v>
       </c>
@@ -27742,7 +27739,7 @@
         <v>0.60069444444444442</v>
       </c>
       <c r="D308" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E308" s="19">
         <v>3</v>
@@ -27802,7 +27799,7 @@
         <v>5</v>
       </c>
       <c r="Z308" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA308" s="46" t="s">
         <v>91</v>
@@ -27851,7 +27848,7 @@
       <c r="BM308" s="51"/>
       <c r="BN308" s="51"/>
     </row>
-    <row r="309" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A309" s="19"/>
       <c r="B309" s="39"/>
       <c r="C309" s="40"/>
@@ -27916,7 +27913,7 @@
       <c r="BM309" s="51"/>
       <c r="BN309" s="51"/>
     </row>
-    <row r="310" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A310" s="19" t="s">
         <v>7</v>
       </c>
@@ -27927,7 +27924,7 @@
         <v>0.60069444444444442</v>
       </c>
       <c r="D310" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E310" s="19">
         <v>3</v>
@@ -27960,7 +27957,7 @@
         <v>579</v>
       </c>
       <c r="O310" s="45" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P310" s="46" t="s">
         <v>22</v>
@@ -27969,7 +27966,7 @@
         <v>105</v>
       </c>
       <c r="R310" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="S310" s="19"/>
       <c r="T310" s="20">
@@ -27987,7 +27984,7 @@
         <v>5</v>
       </c>
       <c r="Z310" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA310" s="46" t="s">
         <v>91</v>
@@ -28036,7 +28033,7 @@
       <c r="BM310" s="51"/>
       <c r="BN310" s="51"/>
     </row>
-    <row r="311" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A311" s="19"/>
       <c r="B311" s="39"/>
       <c r="C311" s="40"/>
@@ -28101,7 +28098,7 @@
       <c r="BM311" s="51"/>
       <c r="BN311" s="51"/>
     </row>
-    <row r="312" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A312" s="19"/>
       <c r="B312" s="39"/>
       <c r="C312" s="40"/>
@@ -28166,7 +28163,7 @@
       <c r="BM312" s="51"/>
       <c r="BN312" s="51"/>
     </row>
-    <row r="313" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A313" s="19" t="s">
         <v>7</v>
       </c>
@@ -28177,7 +28174,7 @@
         <v>0.60069444444444442</v>
       </c>
       <c r="D313" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E313" s="19">
         <v>3</v>
@@ -28210,7 +28207,7 @@
         <v>610</v>
       </c>
       <c r="O313" s="45" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P313" s="46" t="s">
         <v>22</v>
@@ -28219,7 +28216,7 @@
         <v>105</v>
       </c>
       <c r="R313" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S313" s="19"/>
       <c r="T313" s="20">
@@ -28237,7 +28234,7 @@
         <v>5</v>
       </c>
       <c r="Z313" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA313" s="46" t="s">
         <v>91</v>
@@ -28286,7 +28283,7 @@
       <c r="BM313" s="51"/>
       <c r="BN313" s="51"/>
     </row>
-    <row r="314" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A314" s="19"/>
       <c r="B314" s="39"/>
       <c r="C314" s="40"/>
@@ -28351,7 +28348,7 @@
       <c r="BM314" s="51"/>
       <c r="BN314" s="51"/>
     </row>
-    <row r="315" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A315" s="19"/>
       <c r="B315" s="39"/>
       <c r="C315" s="40"/>
@@ -28416,7 +28413,7 @@
       <c r="BM315" s="51"/>
       <c r="BN315" s="51"/>
     </row>
-    <row r="316" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A316" s="19" t="s">
         <v>7</v>
       </c>
@@ -28427,7 +28424,7 @@
         <v>0.60069444444444442</v>
       </c>
       <c r="D316" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E316" s="19">
         <v>3</v>
@@ -28460,7 +28457,7 @@
         <v>1935</v>
       </c>
       <c r="O316" s="45" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P316" s="46" t="s">
         <v>22</v>
@@ -28469,7 +28466,7 @@
         <v>210</v>
       </c>
       <c r="R316" s="19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="S316" s="19"/>
       <c r="T316" s="20">
@@ -28487,7 +28484,7 @@
         <v>5</v>
       </c>
       <c r="Z316" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA316" s="46" t="s">
         <v>91</v>
@@ -28536,7 +28533,7 @@
       <c r="BM316" s="51"/>
       <c r="BN316" s="51"/>
     </row>
-    <row r="317" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A317" s="19"/>
       <c r="B317" s="39"/>
       <c r="C317" s="40"/>
@@ -28601,7 +28598,7 @@
       <c r="BM317" s="51"/>
       <c r="BN317" s="51"/>
     </row>
-    <row r="318" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A318" s="19"/>
       <c r="B318" s="39"/>
       <c r="C318" s="40"/>
@@ -28666,7 +28663,7 @@
       <c r="BM318" s="51"/>
       <c r="BN318" s="51"/>
     </row>
-    <row r="319" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A319" s="19" t="s">
         <v>7</v>
       </c>
@@ -28677,7 +28674,7 @@
         <v>0.60069444444444442</v>
       </c>
       <c r="D319" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E319" s="19">
         <v>3</v>
@@ -28741,7 +28738,7 @@
         <v>56</v>
       </c>
       <c r="Z319" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA319" s="46" t="s">
         <v>91</v>
@@ -28862,7 +28859,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="320" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A320" s="19" t="s">
         <v>7</v>
       </c>
@@ -28873,7 +28870,7 @@
         <v>0.59027777777777801</v>
       </c>
       <c r="D320" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E320" s="19">
         <v>3</v>
@@ -28906,7 +28903,7 @@
         <v>175</v>
       </c>
       <c r="O320" s="46" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P320" s="46" t="s">
         <v>22</v>
@@ -28915,7 +28912,7 @@
         <v>99</v>
       </c>
       <c r="R320" s="19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="S320" s="19"/>
       <c r="T320" s="20">
@@ -28933,7 +28930,7 @@
         <v>5</v>
       </c>
       <c r="Z320" s="46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AA320" s="46" t="s">
         <v>91</v>
@@ -28982,7 +28979,7 @@
       <c r="BM320" s="51"/>
       <c r="BN320" s="51"/>
     </row>
-    <row r="321" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A321" s="19"/>
       <c r="B321" s="39"/>
       <c r="C321" s="40"/>
@@ -29046,7 +29043,7 @@
       <c r="BM321" s="51"/>
       <c r="BN321" s="51"/>
     </row>
-    <row r="322" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A322" s="19" t="s">
         <v>7</v>
       </c>
@@ -29057,7 +29054,7 @@
         <v>0.59027777777777801</v>
       </c>
       <c r="D322" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E322" s="19">
         <v>3</v>
@@ -29117,7 +29114,7 @@
         <v>5</v>
       </c>
       <c r="Z322" s="46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AA322" s="46" t="s">
         <v>91</v>
@@ -29172,7 +29169,7 @@
       <c r="BM322" s="51"/>
       <c r="BN322" s="51"/>
     </row>
-    <row r="323" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A323" s="19"/>
       <c r="B323" s="39"/>
       <c r="C323" s="40"/>
@@ -29243,7 +29240,7 @@
       <c r="BM323" s="51"/>
       <c r="BN323" s="51"/>
     </row>
-    <row r="324" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A324" s="19" t="s">
         <v>7</v>
       </c>
@@ -29254,7 +29251,7 @@
         <v>0.59027777777777801</v>
       </c>
       <c r="D324" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E324" s="19">
         <v>3</v>
@@ -29287,13 +29284,13 @@
         <v>1837</v>
       </c>
       <c r="O324" s="45" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P324" s="46" t="s">
         <v>22</v>
       </c>
       <c r="Q324" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="R324" s="19" t="s">
         <v>51</v>
@@ -29314,7 +29311,7 @@
         <v>5</v>
       </c>
       <c r="Z324" s="46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AA324" s="46" t="s">
         <v>91</v>
@@ -29363,7 +29360,7 @@
       <c r="BM324" s="51"/>
       <c r="BN324" s="51"/>
     </row>
-    <row r="325" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A325" s="19"/>
       <c r="B325" s="39"/>
       <c r="C325" s="40"/>
@@ -29428,7 +29425,7 @@
       <c r="BM325" s="51"/>
       <c r="BN325" s="51"/>
     </row>
-    <row r="326" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:66" s="46" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A326" s="19" t="s">
         <v>7</v>
       </c>
@@ -29439,7 +29436,7 @@
         <v>0.59027777777777801</v>
       </c>
       <c r="D326" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E326" s="19">
         <v>3</v>
@@ -29503,7 +29500,7 @@
         <v>56</v>
       </c>
       <c r="Z326" s="46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AA326" s="46" t="s">
         <v>91</v>
@@ -29624,7 +29621,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="327" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A327" s="47"/>
       <c r="B327" s="54"/>
       <c r="C327" s="47"/>
@@ -29681,7 +29678,7 @@
       <c r="BM327" s="51"/>
       <c r="BN327" s="51"/>
     </row>
-    <row r="328" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A328" s="47"/>
       <c r="B328" s="54"/>
       <c r="C328" s="47"/>
@@ -29738,7 +29735,7 @@
       <c r="BM328" s="51"/>
       <c r="BN328" s="51"/>
     </row>
-    <row r="329" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A329" s="47"/>
       <c r="B329" s="54"/>
       <c r="C329" s="47"/>
@@ -29795,7 +29792,7 @@
       <c r="BM329" s="51"/>
       <c r="BN329" s="51"/>
     </row>
-    <row r="330" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A330" s="47"/>
       <c r="B330" s="54"/>
       <c r="C330" s="47"/>
@@ -29861,6 +29858,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E832286978553240BFB7D21D3C3651DD" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c1b20562b99f7fe99bf60d309995437">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92d8d115-32c9-434a-b663-4c72c8f3681a" xmlns:ns3="bd451e3b-750f-4bd1-994b-00bb98b93a1b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c37cacaf12cf73f41a70ef15741328a" ns2:_="" ns3:_="">
     <xsd:import namespace="92d8d115-32c9-434a-b663-4c72c8f3681a"/>
@@ -30043,15 +30049,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -30059,13 +30056,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B9984A3-1547-4B62-8D85-E11EA4491641}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EC1564F-335F-4B8D-9A63-77F1686BCF21}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EC1564F-335F-4B8D-9A63-77F1686BCF21}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B9984A3-1547-4B62-8D85-E11EA4491641}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="92d8d115-32c9-434a-b663-4c72c8f3681a"/>
+    <ds:schemaRef ds:uri="bd451e3b-750f-4bd1-994b-00bb98b93a1b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A1B77A4-ACF5-4802-997A-EEB8D1D1989A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A1B77A4-ACF5-4802-997A-EEB8D1D1989A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>